<commit_message>
code 정리 및 PlayerInfoView 기능 추가
</commit_message>
<xml_diff>
--- a/GameData/HandRankingStat.xlsx
+++ b/GameData/HandRankingStat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BalatroP\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wook\Documents\GitHub\BalatroP\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25404" windowHeight="13248"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="5028"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,51 +46,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RoyalFlush</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flush</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IncreaseChip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>IncreaseDrainage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRIPLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROYAL FLUSH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOUR CARD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FULL HOUSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIVE CARD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FlUSH FIVE CARD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HIGH CARD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ONE PAIR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWO PAIR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STRAIGHT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLUSH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STRAIGHT FLUSH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -488,122 +496,122 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1">
-        <v>180</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="D3" s="1">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="G3" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
         <v>50</v>
       </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>22</v>
-      </c>
       <c r="G4" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D6" s="1">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
@@ -611,22 +619,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>350</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D7" s="1">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1">
         <v>4</v>
@@ -634,22 +642,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="D8" s="1">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1">
         <v>4</v>
@@ -657,22 +665,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>450</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1">
         <v>4</v>
@@ -680,48 +688,94 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1">
-        <v>110</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
-        <v>550</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="D11" s="1">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
         <v>20</v>
       </c>
       <c r="G11" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>